<commit_message>
approved by tech lead
</commit_message>
<xml_diff>
--- a/SimpCity US13 Test Case (Not Checked).xlsx
+++ b/SimpCity US13 Test Case (Not Checked).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Test Cases (Not Checked)\Sprint 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claris Toh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF802ACC-D71D-4B7E-9F61-706BE808A574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7164F4A9-1B35-406B-8F80-838E7227F15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27930" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US13 Sprint 4 " sheetId="23" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>The program will processed the chosen option as accordance to the functionality of the chosen option.</t>
   </si>
   <si>
-    <t>US13 - As a user, I would like to only be able to enter a number for choices so that I do not get confused.</t>
-  </si>
-  <si>
     <t>Mr Low</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   <si>
     <t>1. The users enters an invalid input that is not a numeric interger when the message "Your Choice?" is prompted.
 Eg --&gt; Your Choice? aaa</t>
+  </si>
+  <si>
+    <t>US13 - As a user, I would like to only be able to enter a number of choices so that I do not get confused.</t>
   </si>
 </sst>
 </file>
@@ -1107,6 +1107,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1147,21 +1162,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1481,7 +1481,7 @@
   <dimension ref="A1:AO24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,10 +1500,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="121"/>
+      <c r="C1" s="107"/>
       <c r="D1" s="40"/>
       <c r="E1" s="38"/>
       <c r="F1" s="42"/>
@@ -1516,24 +1516,24 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="122"/>
+      <c r="C2" s="108"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="118" t="s">
+      <c r="E2" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="122"/>
+      <c r="F2" s="108"/>
       <c r="G2" s="86"/>
-      <c r="H2" s="122" t="s">
+      <c r="H2" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="118" t="s">
+      <c r="I2" s="108"/>
+      <c r="J2" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="119"/>
+      <c r="K2" s="105"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="44" t="s">
@@ -1586,7 +1586,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="32" t="s">
         <v>14</v>
@@ -1654,20 +1654,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="120" t="s">
+      <c r="B7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="120"/>
+      <c r="C7" s="106"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="120" t="s">
+      <c r="E7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="120"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="87"/>
-      <c r="H7" s="120" t="s">
+      <c r="H7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="120"/>
+      <c r="I7" s="106"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -1677,7 +1677,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="62" t="s">
@@ -1798,40 +1798,40 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="68" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="104">
+      <c r="A14" s="109">
         <v>1</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="110" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="D14" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="111"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="116"/>
       <c r="I14" s="83"/>
       <c r="J14" s="83"/>
       <c r="K14" s="84"/>
     </row>
     <row r="15" spans="1:12" ht="319.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="82" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="112" t="s">
+      <c r="F15" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="115" t="s">
+      <c r="G15" s="120" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="77" t="s">
@@ -1846,19 +1846,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="97" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="D16" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="E16" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="97" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="113"/>
-      <c r="G16" s="116"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="102" t="s">
         <v>41</v>
       </c>
@@ -1871,19 +1871,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="D17" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="80" t="s">
-        <v>57</v>
-      </c>
       <c r="E17" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="114"/>
-      <c r="G17" s="117"/>
+        <v>53</v>
+      </c>
+      <c r="F17" s="119"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="77" t="s">
         <v>41</v>
       </c>
@@ -2015,6 +2015,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
@@ -2023,13 +2030,6 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F15 F18" xr:uid="{9283E15E-2C36-477F-92C5-9CFF3B72F83D}">

</xml_diff>